<commit_message>
Fixed bug in finder which dramatically lowered KU if on multiple "health" defines with less than "1" KU. Fixed climate duplicates
</commit_message>
<xml_diff>
--- a/ExpertSystem/files/climate.xlsx
+++ b/ExpertSystem/files/climate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="52">
   <si>
     <t>Россия</t>
   </si>
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,17 +961,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>